<commit_message>
register fix + individdual attendance
fixed regex for password + self attendance sheet
</commit_message>
<xml_diff>
--- a/server/storage/individual-template.xlsx
+++ b/server/storage/individual-template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\sms-qr\server\storage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7896C7-3F11-4A94-A349-93BB0744B57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF3E776-1CD3-459D-9CD4-85505BF8D3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2505" yWindow="2505" windowWidth="18000" windowHeight="9270" xr2:uid="{8E0A1244-566C-4285-B8A1-3C25EEBF0295}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Attendance" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -173,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -317,40 +317,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -377,19 +351,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -518,6 +479,47 @@
         <color indexed="64"/>
       </left>
       <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -525,9 +527,46 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -538,9 +577,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -552,71 +589,6 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -630,7 +602,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,21 +620,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -683,19 +655,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -722,91 +694,106 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1126,7 +1113,7 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C1:I3"/>
+      <selection activeCell="D3" sqref="D3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,64 +1128,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="52" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
+      <c r="H1" s="58"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="56"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="37"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="48" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="49"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="59"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="40"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="63"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="60"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="51"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="62"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="43"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -1217,24 +1204,24 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
     </row>
     <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
+      <c r="B6" s="54"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
+      <c r="G6" s="54"/>
+      <c r="H6" s="54"/>
     </row>
     <row r="7" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
@@ -1260,13 +1247,13 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="46"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="46"/>
       <c r="J8" s="27" t="s">
         <v>13</v>
       </c>
@@ -1276,12 +1263,12 @@
     </row>
     <row r="9" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="25"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="44"/>
       <c r="J9" s="30" t="s">
         <v>14</v>
       </c>
@@ -1291,93 +1278,93 @@
     </row>
     <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="25"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="44"/>
     </row>
     <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="25"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="44"/>
     </row>
     <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="25"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="44"/>
     </row>
     <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="25"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="44"/>
     </row>
     <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="25"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="44"/>
     </row>
     <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="25"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="44"/>
     </row>
     <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="25"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="44"/>
     </row>
     <row r="17" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="25"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="44"/>
     </row>
     <row r="18" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="25"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="44"/>
     </row>
     <row r="19" spans="2:10" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="26"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="45"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
@@ -1430,10 +1417,12 @@
     </row>
   </sheetData>
   <mergeCells count="64">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="D2:I2"/>
+    <mergeCell ref="D3:I3"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="B5:H6"/>
     <mergeCell ref="B8:B9"/>
@@ -1442,9 +1431,7 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="G8:G9"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="A1:C1"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="D12:D13"/>

</xml_diff>